<commit_message>
Users Report Creation facilitated
</commit_message>
<xml_diff>
--- a/Users_Report.xlsx
+++ b/Users_Report.xlsx
@@ -1,3 +1,60 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users_Report" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -280,4 +337,158 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>User Email ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total no. of Posts</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>No. of times Reported</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_staff</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anshal</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>shukla.anshal85@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f20190363@pilani.bits-pilani.ac.in</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>shukla.anshal85</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>shukla.anshal85@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>f20190363</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>f20190363@pilani.bits-pilani.ac.in</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Image Resize and Redirection
</commit_message>
<xml_diff>
--- a/Users_Report.xlsx
+++ b/Users_Report.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,12 +393,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -474,15 +474,42 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sambhav</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>f20190192@pilani.bits-pilani.ac.in</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>